<commit_message>
versjon av dokumentasjon som ble brukt under presentasjon av concept0
</commit_message>
<xml_diff>
--- a/doc/le_nb_iot_controller_current_consumption.xlsx
+++ b/doc/le_nb_iot_controller_current_consumption.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9090" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9090"/>
   </bookViews>
   <sheets>
-    <sheet name="current and cost" sheetId="1" r:id="rId1"/>
+    <sheet name="current and lifetime" sheetId="1" r:id="rId1"/>
     <sheet name="data format and storage" sheetId="2" r:id="rId2"/>
     <sheet name="ADC measurements" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="185">
   <si>
     <t>function</t>
   </si>
@@ -251,15 +251,6 @@
   </si>
   <si>
     <t>M95</t>
-  </si>
-  <si>
-    <t>certification (IPX)</t>
-  </si>
-  <si>
-    <t>production startup (Noca)</t>
-  </si>
-  <si>
-    <t>external lab testing (EM interference in Swe)</t>
   </si>
   <si>
     <t>measurement</t>
@@ -295,30 +286,6 @@
 It's the same rate that data is stored to the external memory.</t>
   </si>
   <si>
-    <t>load cell (AMEKA)</t>
-  </si>
-  <si>
-    <t>total cost  com module</t>
-  </si>
-  <si>
-    <t>total cost load cell module</t>
-  </si>
-  <si>
-    <t>unit cost load cell + com module</t>
-  </si>
-  <si>
-    <t>com module (AMEKA)</t>
-  </si>
-  <si>
-    <t>including additional CAD work, roughly est 50-70k per unit.</t>
-  </si>
-  <si>
-    <t>build by three pieces.</t>
-  </si>
-  <si>
-    <t>tbd</t>
-  </si>
-  <si>
     <t>Radio average</t>
   </si>
   <si>
@@ -326,9 +293,6 @@
   </si>
   <si>
     <t>sensor + Radio average total</t>
-  </si>
-  <si>
-    <t>total cost  com module for pilot</t>
   </si>
   <si>
     <t>Analog Dev.</t>
@@ -624,6 +588,18 @@
   </si>
   <si>
     <t>tiny13a?</t>
+  </si>
+  <si>
+    <t>MQTT topic</t>
+  </si>
+  <si>
+    <t>LE</t>
+  </si>
+  <si>
+    <t>A lot of Tx and Rx during power up due to re-connection to network and open TCP socket towards server.</t>
+  </si>
+  <si>
+    <t>Assuming only one startup, then wakeup from sleep is faster than power up. Need to be confirmed.</t>
   </si>
 </sst>
 </file>
@@ -686,7 +662,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -761,43 +737,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -818,7 +757,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -841,13 +780,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -856,11 +788,14 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -1180,9 +1115,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:L81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="14" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="14" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1195,47 +1130,51 @@
     <col min="6" max="6" width="23" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.3984375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="56.1328125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="8.86328125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1328125" style="1"/>
+    <col min="9" max="9" width="8.86328125" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="12" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="4">
+      <c r="B2" s="7"/>
+      <c r="C2" s="8">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="23" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="1">
+      <c r="B3" s="18"/>
+      <c r="C3" s="18">
         <v>2E-3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="24" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="4">
+      <c r="B4" s="11"/>
+      <c r="C4" s="12">
         <v>600</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="25" t="s">
         <v>6</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
@@ -1246,7 +1185,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>50</v>
       </c>
@@ -1260,9 +1199,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C7" s="1">
         <v>0.1</v>
@@ -1271,10 +1210,10 @@
         <v>6</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="71.25" x14ac:dyDescent="0.45">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="71.25" hidden="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>69</v>
       </c>
@@ -1285,10 +1224,11 @@
         <v>6</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1297,7 +1237,7 @@
         <v>4.0000000000000002E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1306,7 +1246,7 @@
         <v>1.6666666666666667E-5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>40</v>
       </c>
@@ -1315,18 +1255,18 @@
         <v>1.6666666666666667E-6</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C13" s="1">
         <f>C7/C4</f>
         <v>1.6666666666666669E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C14" s="1">
         <f>C8/C4</f>
@@ -1342,7 +1282,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="57" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" ht="57" hidden="1" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -1352,11 +1292,11 @@
       <c r="D15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H15" s="19" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="H15" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>59</v>
       </c>
@@ -1370,7 +1310,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:12" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
         <v>62</v>
       </c>
@@ -1382,10 +1322,10 @@
         <v>20</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="I17" s="1">
         <v>1</v>
@@ -1398,7 +1338,8 @@
         <v>224</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>0</v>
       </c>
@@ -1424,7 +1365,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -1444,7 +1385,7 @@
         <v>0.22</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="I20" s="1">
         <v>1</v>
@@ -1460,7 +1401,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="D21" s="1" t="s">
         <v>18</v>
       </c>
@@ -1471,7 +1412,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="D22" s="1" t="s">
         <v>27</v>
       </c>
@@ -1482,7 +1423,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="D23" s="1" t="s">
         <v>15</v>
       </c>
@@ -1490,7 +1431,7 @@
         <v>5.0000000000000004E-6</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="D24" s="1" t="s">
         <v>26</v>
       </c>
@@ -1501,7 +1442,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="D25" s="1" t="s">
         <v>23</v>
       </c>
@@ -1512,7 +1453,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="D26" s="1" t="s">
         <v>19</v>
       </c>
@@ -1525,7 +1466,7 @@
         <v>38.871904208175479</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
@@ -1539,7 +1480,7 @@
         <v>17</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="F27" s="1">
         <v>0.23400000000000001</v>
@@ -1558,7 +1499,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="D28" s="1" t="s">
         <v>18</v>
       </c>
@@ -1566,7 +1507,7 @@
         <v>0.217</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="D29" s="1" t="s">
         <v>27</v>
       </c>
@@ -1574,7 +1515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="D30" s="1" t="s">
         <v>15</v>
       </c>
@@ -1582,19 +1523,19 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:12" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
       <c r="D31" s="1" t="s">
         <v>26</v>
       </c>
       <c r="F31" s="1">
         <v>1.4999999999999999E-4</v>
       </c>
-      <c r="H31" s="19" t="s">
+      <c r="H31" s="14" t="s">
         <v>68</v>
       </c>
       <c r="I31"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
       <c r="D32" s="1" t="s">
         <v>23</v>
       </c>
@@ -1602,33 +1543,39 @@
         <v>2.1999999999999999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D33" s="1" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="F33" s="1">
-        <f>F31+(F32*$C$13)+(F27*$C$11)+(F29*$C$12)+(F32*C14)</f>
-        <v>1.2609000000000001E-3</v>
+        <f>F31+(F32*$C$13)+(F27*$C$11)+(F29*$C$12)+(F27*C14)</f>
+        <v>1.1860900000000002E-2</v>
       </c>
       <c r="G33" s="1">
         <f>$C$17/F33/24/365</f>
-        <v>0.48298292166554235</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+        <v>5.1344599982133088E-2</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D34" s="1" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="F34" s="1">
-        <f>F30+(F32*$C$13)+(F27*$C$11)+(F29*$C$12)+(F32*C14)</f>
-        <v>2.4108999999999997E-3</v>
+        <f>F30+(F32*$C$13)+(F27*$C$11)+(F29*$C$12)</f>
+        <v>1.3108999999999998E-3</v>
       </c>
       <c r="G34" s="1">
         <f>$C$17/F34/24/365</f>
-        <v>0.25259992779795204</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+        <v>0.46456111520946108</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>30</v>
       </c>
@@ -1661,7 +1608,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="D36" s="1" t="s">
         <v>57</v>
       </c>
@@ -1669,7 +1616,7 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="D37" s="1" t="s">
         <v>35</v>
       </c>
@@ -1677,7 +1624,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="D38" s="1" t="s">
         <v>36</v>
       </c>
@@ -1685,7 +1632,7 @@
         <v>7.9999999999999996E-6</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="D39" s="1" t="s">
         <v>19</v>
       </c>
@@ -1698,7 +1645,7 @@
         <v>101.13925474890652</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>45</v>
       </c>
@@ -1731,7 +1678,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="D41" s="1" t="s">
         <v>25</v>
       </c>
@@ -1739,7 +1686,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="D42" s="1" t="s">
         <v>19</v>
       </c>
@@ -1752,7 +1699,7 @@
         <v>120.59270612437275</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>51</v>
       </c>
@@ -1786,7 +1733,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="D44" s="1" t="s">
         <v>19</v>
       </c>
@@ -1798,11 +1745,11 @@
         <f>$C$17/F44/24/365</f>
         <v>94908.02585892193</v>
       </c>
-      <c r="H44" s="22" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="114" x14ac:dyDescent="0.45">
+      <c r="H44" s="17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="114" hidden="1" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>63</v>
       </c>
@@ -1821,11 +1768,11 @@
       <c r="F45" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="H45" s="19" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="H45" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="D46" s="1" t="s">
         <v>19</v>
       </c>
@@ -1838,9 +1785,9 @@
         <v>304.49658296404118</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>19</v>
@@ -1853,21 +1800,21 @@
         <v>30.449658296404117</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="F48" s="1">
         <v>3.9999999999999998E-6</v>
@@ -1877,21 +1824,21 @@
         <v>152.24829148202065</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>19</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="F49" s="1">
         <v>5.0000000000000004E-6</v>
@@ -1901,20 +1848,21 @@
         <v>121.79863318561647</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>3</v>
@@ -1923,16 +1871,16 @@
         <v>23</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="F52" s="1">
         <v>1.2999999999999999E-5</v>
       </c>
-      <c r="H52" s="19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="H52" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="D53" s="1" t="s">
         <v>15</v>
       </c>
@@ -1940,7 +1888,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="D54" s="1" t="s">
         <v>19</v>
       </c>
@@ -1953,7 +1901,10 @@
         <v>46.845628148314034</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.45"/>
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="D58" s="1" t="s">
         <v>67</v>
       </c>
@@ -1966,9 +1917,9 @@
         <v>46.567120944205421</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="D59" s="1" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="F59" s="1">
         <f>F26+F39+F42+F44</f>
@@ -1982,22 +1933,22 @@
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="F60" s="1">
         <f>F33+F39+F42+F44</f>
-        <v>1.2719777500000001E-3</v>
+        <v>1.1871977750000002E-2</v>
       </c>
       <c r="G60" s="1">
         <f>$C$17/F60/24/365</f>
-        <v>0.47877658703391818</v>
+        <v>5.1296690303187474E-2</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="D61" s="1" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="F61" s="1">
         <f>F20+F25+F36+F37+F41+F43+F45</f>
@@ -2007,7 +1958,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.45">
       <c r="F62" s="1">
         <f>F27+F32+F36+F37+F41+F43+F45</f>
         <v>0.26843500000000003</v>
@@ -2018,7 +1969,7 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.45">
       <c r="D63" s="6" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="E63" s="7"/>
       <c r="F63" s="7">
@@ -2038,18 +1989,18 @@
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="D64" s="25"/>
-      <c r="E64" s="23"/>
-      <c r="F64" s="23">
+      <c r="D64" s="20"/>
+      <c r="E64" s="18"/>
+      <c r="F64" s="18">
         <f>F33+F39+F42+F44+F46+F47</f>
-        <v>1.2939777500000002E-3</v>
-      </c>
-      <c r="G64" s="24">
+        <v>1.1893977750000001E-2</v>
+      </c>
+      <c r="G64" s="19">
         <f>$C$17/F64/24/365</f>
-        <v>0.4706365050929836</v>
-      </c>
-      <c r="H64" s="26" t="s">
-        <v>169</v>
+        <v>5.1201808068632247E-2</v>
+      </c>
+      <c r="H64" s="21" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.45">
@@ -2057,202 +2008,197 @@
       <c r="E65" s="11"/>
       <c r="F65" s="11">
         <f>F34+F39+F42+F44+F46+F47</f>
-        <v>2.4439777499999996E-3</v>
+        <v>1.3439777499999999E-3</v>
       </c>
       <c r="G65" s="12">
         <f>$C$17/F65/24/365</f>
-        <v>0.24918114165649935</v>
+        <v>0.45312741667641632</v>
       </c>
       <c r="H65" s="13" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A68" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="I68" s="1">
-        <v>1</v>
-      </c>
-      <c r="J68" s="1">
-        <v>10000</v>
-      </c>
-      <c r="K68" s="1">
-        <f>I68*J68</f>
-        <v>10000</v>
-      </c>
+      <c r="A68"/>
+      <c r="B68"/>
+      <c r="C68"/>
+      <c r="D68"/>
+      <c r="E68"/>
+      <c r="F68"/>
+      <c r="G68"/>
+      <c r="H68"/>
+      <c r="I68"/>
+      <c r="J68"/>
+      <c r="K68"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A69" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I69" s="1">
-        <v>1</v>
-      </c>
-      <c r="J69" s="1">
-        <v>20000</v>
-      </c>
-      <c r="K69" s="1">
-        <f>I69*J69</f>
-        <v>20000</v>
-      </c>
+      <c r="A69"/>
+      <c r="B69"/>
+      <c r="C69"/>
+      <c r="D69"/>
+      <c r="E69"/>
+      <c r="F69"/>
+      <c r="G69"/>
+      <c r="H69"/>
+      <c r="I69"/>
+      <c r="J69"/>
+      <c r="K69"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A70" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I70" s="1">
-        <v>1</v>
-      </c>
-      <c r="J70" s="1">
-        <v>100000</v>
-      </c>
-      <c r="K70" s="1">
-        <f>I70*J70</f>
-        <v>100000</v>
-      </c>
+      <c r="A70"/>
+      <c r="B70"/>
+      <c r="C70"/>
+      <c r="D70"/>
+      <c r="E70"/>
+      <c r="F70"/>
+      <c r="G70"/>
+      <c r="H70"/>
+      <c r="I70"/>
+      <c r="J70"/>
+      <c r="K70"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A71" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H71" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="I71" s="1">
-        <v>1</v>
-      </c>
-      <c r="J71" s="1">
-        <v>100000</v>
-      </c>
-      <c r="K71" s="1">
-        <f>I71*J71</f>
-        <v>100000</v>
-      </c>
+      <c r="A71"/>
+      <c r="B71"/>
+      <c r="C71"/>
+      <c r="D71"/>
+      <c r="E71"/>
+      <c r="F71"/>
+      <c r="G71"/>
+      <c r="H71"/>
+      <c r="I71"/>
+      <c r="J71"/>
+      <c r="K71"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A72" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="I72" s="4">
-        <v>1</v>
-      </c>
-      <c r="J72" s="4">
-        <f>(K63)+((K68+K69+K70+K71)/I72)</f>
-        <v>230631</v>
-      </c>
-      <c r="K72" s="1">
-        <f>(K68+K69+K70+K71)*I72</f>
-        <v>230000</v>
-      </c>
+      <c r="A72"/>
+      <c r="B72"/>
+      <c r="C72"/>
+      <c r="D72"/>
+      <c r="E72"/>
+      <c r="F72"/>
+      <c r="G72"/>
+      <c r="H72"/>
+      <c r="I72"/>
+      <c r="J72"/>
+      <c r="K72"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A73" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="A73"/>
+      <c r="B73"/>
+      <c r="C73"/>
+      <c r="D73"/>
+      <c r="E73"/>
+      <c r="F73"/>
+      <c r="G73"/>
+      <c r="H73"/>
       <c r="I73"/>
       <c r="J73"/>
+      <c r="K73"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A74"/>
+      <c r="B74"/>
+      <c r="C74"/>
+      <c r="D74"/>
+      <c r="E74"/>
+      <c r="F74"/>
+      <c r="G74"/>
+      <c r="H74"/>
+      <c r="I74"/>
+      <c r="J74"/>
+      <c r="K74"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A75" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H75" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="I75" s="1">
-        <v>1</v>
-      </c>
-      <c r="J75" s="1">
-        <v>100000</v>
-      </c>
-      <c r="K75" s="1">
-        <f>I75*J75</f>
-        <v>100000</v>
-      </c>
+      <c r="A75"/>
+      <c r="B75"/>
+      <c r="C75"/>
+      <c r="D75"/>
+      <c r="E75"/>
+      <c r="F75"/>
+      <c r="G75"/>
+      <c r="H75"/>
+      <c r="I75"/>
+      <c r="J75"/>
+      <c r="K75"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A76" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="I76" s="1">
-        <v>1</v>
-      </c>
-      <c r="J76" s="1">
-        <v>20000</v>
-      </c>
-      <c r="K76" s="1">
-        <f>I76*J76</f>
-        <v>20000</v>
-      </c>
+      <c r="A76"/>
+      <c r="B76"/>
+      <c r="C76"/>
+      <c r="D76"/>
+      <c r="E76"/>
+      <c r="F76"/>
+      <c r="G76"/>
+      <c r="H76"/>
+      <c r="I76"/>
+      <c r="J76"/>
+      <c r="K76"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A77" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I77" s="1">
-        <v>1</v>
-      </c>
-      <c r="J77" s="1">
-        <v>100000</v>
-      </c>
-      <c r="K77" s="1">
-        <f>I77*J77</f>
-        <v>100000</v>
-      </c>
+      <c r="A77"/>
+      <c r="B77"/>
+      <c r="C77"/>
+      <c r="D77"/>
+      <c r="E77"/>
+      <c r="F77"/>
+      <c r="G77"/>
+      <c r="H77"/>
+      <c r="I77"/>
+      <c r="J77"/>
+      <c r="K77"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A78" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H78" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="I78" s="1">
-        <v>1</v>
-      </c>
-      <c r="J78" s="1">
-        <v>100000</v>
-      </c>
-      <c r="K78" s="1">
-        <f>I78*J78</f>
-        <v>100000</v>
-      </c>
+      <c r="A78"/>
+      <c r="B78"/>
+      <c r="C78"/>
+      <c r="D78"/>
+      <c r="E78"/>
+      <c r="F78"/>
+      <c r="G78"/>
+      <c r="H78"/>
+      <c r="I78"/>
+      <c r="J78"/>
+      <c r="K78"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A79" s="1" t="s">
-        <v>90</v>
-      </c>
+      <c r="A79"/>
+      <c r="B79"/>
+      <c r="C79"/>
+      <c r="D79"/>
+      <c r="E79"/>
+      <c r="F79"/>
+      <c r="G79"/>
+      <c r="H79"/>
       <c r="I79"/>
-      <c r="J79" s="4">
-        <f>(K63)+((K75+K76+K77+K78)/I72)</f>
-        <v>320631</v>
-      </c>
-      <c r="K79" s="1">
-        <f>(K75+K76+K77+K78)*I72</f>
-        <v>320000</v>
-      </c>
+      <c r="J79"/>
+      <c r="K79"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A80"/>
+      <c r="B80"/>
+      <c r="C80"/>
+      <c r="D80"/>
+      <c r="E80"/>
+      <c r="F80"/>
+      <c r="G80"/>
+      <c r="H80"/>
+      <c r="I80"/>
+      <c r="J80"/>
+      <c r="K80"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A81" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="B81" s="15"/>
-      <c r="C81" s="15"/>
-      <c r="D81" s="15"/>
-      <c r="E81" s="15"/>
-      <c r="F81" s="15"/>
-      <c r="G81" s="15"/>
-      <c r="H81" s="16"/>
-      <c r="I81" s="15"/>
-      <c r="J81" s="17">
-        <f>J72+J79</f>
-        <v>551262</v>
-      </c>
-      <c r="K81" s="18"/>
+      <c r="A81"/>
+      <c r="B81"/>
+      <c r="C81"/>
+      <c r="D81"/>
+      <c r="E81"/>
+      <c r="F81"/>
+      <c r="G81"/>
+      <c r="H81"/>
+      <c r="I81"/>
+      <c r="J81"/>
+      <c r="K81"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2262,593 +2208,648 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="10.73046875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.3984375" customWidth="1"/>
-    <col min="7" max="7" width="43.1328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="57.265625" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.3984375" customWidth="1"/>
+    <col min="8" max="8" width="43.1328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="57.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>136</v>
+        <v>181</v>
       </c>
       <c r="B1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>114</v>
       </c>
       <c r="D1" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="E1" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="F1" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="G1" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="H1" t="s">
-        <v>163</v>
+        <v>115</v>
       </c>
       <c r="I1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="J1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A2">
+        <v>133</v>
+      </c>
+      <c r="K1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>116</v>
-      </c>
       <c r="C2" t="s">
-        <v>146</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>151</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
+        <v>134</v>
+      </c>
+      <c r="E2" t="s">
+        <v>139</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>132</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <f>I2</f>
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="L2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J11" si="0">I3</f>
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4" t="s">
+        <v>126</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5" t="s">
+        <v>116</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>182</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>127</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E7" t="s">
+        <v>139</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7" t="s">
+        <v>129</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>182</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" t="s">
+        <v>140</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
         <v>144</v>
       </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
-      <c r="I2">
-        <f>H2</f>
-        <v>2</v>
-      </c>
-      <c r="J2">
+      <c r="H8" t="s">
+        <v>131</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K8">
         <v>4</v>
       </c>
-      <c r="K2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="L8" s="5"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" t="s">
+        <v>134</v>
+      </c>
+      <c r="E9" t="s">
+        <v>140</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>145</v>
+      </c>
+      <c r="H9" t="s">
+        <v>131</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" t="s">
+        <v>135</v>
+      </c>
+      <c r="H10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>182</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" t="s">
+        <v>125</v>
+      </c>
+      <c r="H11" t="s">
+        <v>128</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>4</v>
+      </c>
+      <c r="L11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>182</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
         <v>117</v>
       </c>
-      <c r="C3" t="s">
+      <c r="H12" t="s">
+        <v>131</v>
+      </c>
+      <c r="I12">
+        <v>2</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H13" t="s">
+        <v>131</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>182</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>119</v>
+      </c>
+      <c r="H14" t="s">
+        <v>131</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>182</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>120</v>
+      </c>
+      <c r="H15" t="s">
+        <v>131</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>182</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>121</v>
+      </c>
+      <c r="H16" t="s">
+        <v>131</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>182</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>122</v>
+      </c>
+      <c r="H17" t="s">
+        <v>131</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>182</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>123</v>
+      </c>
+      <c r="H18" t="s">
+        <v>131</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>2</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H20" t="s">
+        <v>98</v>
+      </c>
+      <c r="J20" s="16">
+        <f>SUM(J2:J19)</f>
+        <v>27</v>
+      </c>
+      <c r="K20" s="16">
+        <f>SUM(K2:K19)</f>
+        <v>54</v>
+      </c>
+      <c r="L20" t="s">
         <v>146</v>
       </c>
-      <c r="D3" t="s">
-        <v>151</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>142</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I11" si="0">H3</f>
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D4" t="s">
-        <v>151</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4" t="s">
-        <v>138</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C5" t="s">
-        <v>146</v>
-      </c>
-      <c r="D5" t="s">
-        <v>151</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5" t="s">
-        <v>128</v>
-      </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A6">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C6" t="s">
-        <v>146</v>
-      </c>
-      <c r="D6" t="s">
-        <v>151</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>4</v>
-      </c>
-      <c r="G6" t="s">
-        <v>139</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J6">
-        <v>4</v>
-      </c>
-      <c r="K6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>121</v>
-      </c>
-      <c r="C7" t="s">
-        <v>146</v>
-      </c>
-      <c r="D7" t="s">
-        <v>151</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>5</v>
-      </c>
-      <c r="G7" t="s">
-        <v>141</v>
-      </c>
-      <c r="H7">
-        <v>2</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J7">
-        <v>4</v>
-      </c>
-      <c r="K7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>123</v>
-      </c>
-      <c r="C8" t="s">
-        <v>146</v>
-      </c>
-      <c r="D8" t="s">
-        <v>152</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" t="s">
-        <v>156</v>
-      </c>
-      <c r="G8" t="s">
-        <v>143</v>
-      </c>
-      <c r="H8">
-        <v>2</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J8">
-        <v>4</v>
-      </c>
-      <c r="K8" s="5"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>124</v>
-      </c>
-      <c r="C9" t="s">
-        <v>146</v>
-      </c>
-      <c r="D9" t="s">
-        <v>152</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
-        <v>157</v>
-      </c>
-      <c r="G9" t="s">
-        <v>143</v>
-      </c>
-      <c r="H9">
-        <v>2</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J9">
-        <v>4</v>
-      </c>
-      <c r="K9" s="5"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>125</v>
-      </c>
-      <c r="C10" t="s">
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="C26" t="s">
         <v>147</v>
       </c>
-      <c r="G10" t="s">
-        <v>143</v>
-      </c>
-      <c r="H10">
-        <v>2</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J10">
-        <v>4</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>122</v>
-      </c>
-      <c r="C11" t="s">
-        <v>137</v>
-      </c>
-      <c r="G11" t="s">
-        <v>140</v>
-      </c>
-      <c r="H11">
-        <v>2</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J11">
-        <v>4</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="J26" s="4">
+        <v>10</v>
+      </c>
+      <c r="K26" s="1"/>
+      <c r="L26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="C27" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>129</v>
-      </c>
-      <c r="G12" t="s">
-        <v>143</v>
-      </c>
-      <c r="H12">
-        <v>2</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-      <c r="J12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A13">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>130</v>
-      </c>
-      <c r="G13" t="s">
-        <v>143</v>
-      </c>
-      <c r="H13">
-        <v>2</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
-        <v>2</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="J27" s="4">
+        <f>J20*J26*24*3600/60</f>
+        <v>388800</v>
+      </c>
+      <c r="K27" s="1"/>
+      <c r="L27" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="C28" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A14">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>131</v>
-      </c>
-      <c r="G14" t="s">
-        <v>143</v>
-      </c>
-      <c r="H14">
-        <v>2</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-      <c r="J14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A15">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>132</v>
-      </c>
-      <c r="G15" t="s">
-        <v>143</v>
-      </c>
-      <c r="H15">
-        <v>2</v>
-      </c>
-      <c r="I15">
-        <v>1</v>
-      </c>
-      <c r="J15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A16">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>133</v>
-      </c>
-      <c r="G16" t="s">
-        <v>143</v>
-      </c>
-      <c r="H16">
-        <v>2</v>
-      </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-      <c r="J16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A17">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>134</v>
-      </c>
-      <c r="G17" t="s">
-        <v>143</v>
-      </c>
-      <c r="H17">
-        <v>2</v>
-      </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-      <c r="J17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="A18">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>135</v>
-      </c>
-      <c r="G18" t="s">
-        <v>143</v>
-      </c>
-      <c r="H18">
-        <v>2</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-      <c r="J18">
-        <v>2</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="G20" t="s">
-        <v>110</v>
-      </c>
-      <c r="I20" s="21">
-        <f>SUM(I2:I19)</f>
-        <v>27</v>
-      </c>
-      <c r="J20" s="21">
-        <f>SUM(J2:J19)</f>
-        <v>54</v>
-      </c>
-      <c r="K20" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="B26" t="s">
-        <v>159</v>
-      </c>
-      <c r="I26" s="4">
-        <v>10</v>
-      </c>
-      <c r="J26" s="1"/>
-      <c r="K26" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="B27" t="s">
-        <v>160</v>
-      </c>
-      <c r="I27" s="4">
-        <f>I20*I26*24*3600/60</f>
-        <v>388800</v>
-      </c>
-      <c r="J27" s="1"/>
-      <c r="K27" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="B28" t="s">
-        <v>161</v>
-      </c>
-      <c r="I28" s="4">
+      <c r="J28" s="4">
         <f>(3600*24*365*10)/60</f>
         <v>5256000</v>
       </c>
-      <c r="J28" s="1"/>
-      <c r="K28" t="s">
-        <v>82</v>
+      <c r="K28" s="1"/>
+      <c r="L28" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2861,635 +2862,635 @@
   <dimension ref="A1:V22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.59765625" style="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.86328125" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.265625" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.73046875" style="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.59765625" style="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.59765625" style="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.3984375" style="20" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.1328125" style="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1328125" style="20"/>
+    <col min="1" max="1" width="9.59765625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.86328125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.265625" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.73046875" style="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.59765625" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.59765625" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.3984375" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.1328125" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1328125" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="G1" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="H1" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="I1" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>186</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>187</v>
-      </c>
-      <c r="I1" s="20" t="s">
-        <v>188</v>
-      </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="T1" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="U1" s="20" t="s">
-        <v>108</v>
-      </c>
-      <c r="V1" s="20" t="s">
-        <v>109</v>
+      <c r="T1" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="U1" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="V1" s="15" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A2" s="20">
+      <c r="A2" s="15">
         <v>3.7</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="15">
         <f>A2/1.6</f>
         <v>2.3125</v>
       </c>
-      <c r="C2" s="27">
-        <v>1</v>
-      </c>
-      <c r="D2" s="20">
+      <c r="C2" s="22">
+        <v>1</v>
+      </c>
+      <c r="D2" s="15">
         <v>2.048</v>
       </c>
-      <c r="E2" s="20">
-        <v>1</v>
-      </c>
-      <c r="F2" s="20">
-        <v>2</v>
-      </c>
-      <c r="G2" s="20">
+      <c r="E2" s="15">
+        <v>1</v>
+      </c>
+      <c r="F2" s="15">
+        <v>2</v>
+      </c>
+      <c r="G2" s="15">
         <f>F2/B2/4096</f>
         <v>2.1114864864864866E-4</v>
       </c>
-      <c r="H2" s="20">
+      <c r="H2" s="15">
         <f>F2/C2/4096</f>
         <v>4.8828125E-4</v>
       </c>
-      <c r="I2" s="20">
+      <c r="I2" s="15">
         <f>F2/D2/4096</f>
         <v>2.384185791015625E-4</v>
       </c>
-      <c r="T2" s="20">
+      <c r="T2" s="15">
         <v>3.1970000000000001</v>
       </c>
-      <c r="U2" s="20">
+      <c r="U2" s="15">
         <v>0.99099999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A3" s="20">
+      <c r="A3" s="15">
         <v>3.6</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="15">
         <f t="shared" ref="B3:B17" si="0">A3/1.6</f>
         <v>2.25</v>
       </c>
-      <c r="C3" s="27">
-        <v>1</v>
-      </c>
-      <c r="D3" s="20">
+      <c r="C3" s="22">
+        <v>1</v>
+      </c>
+      <c r="D3" s="15">
         <v>2.048</v>
       </c>
-      <c r="E3" s="20">
-        <v>1</v>
-      </c>
-      <c r="F3" s="20">
-        <v>2</v>
-      </c>
-      <c r="G3" s="20">
+      <c r="E3" s="15">
+        <v>1</v>
+      </c>
+      <c r="F3" s="15">
+        <v>2</v>
+      </c>
+      <c r="G3" s="15">
         <f t="shared" ref="G3:G17" si="1">F3/B3/4096</f>
         <v>2.1701388888888888E-4</v>
       </c>
-      <c r="H3" s="20">
+      <c r="H3" s="15">
         <f t="shared" ref="H3:H17" si="2">F3/C3/4096</f>
         <v>4.8828125E-4</v>
       </c>
-      <c r="I3" s="20">
+      <c r="I3" s="15">
         <f t="shared" ref="I3:I17" si="3">F3/D3/4096</f>
         <v>2.384185791015625E-4</v>
       </c>
-      <c r="T3" s="20">
+      <c r="T3" s="15">
         <v>3.1040000000000001</v>
       </c>
-      <c r="U3" s="20">
+      <c r="U3" s="15">
         <v>0.99099999999999999</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A4" s="20">
+      <c r="A4" s="15">
         <v>3.5</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="15">
         <f t="shared" si="0"/>
         <v>2.1875</v>
       </c>
-      <c r="C4" s="27">
-        <v>1</v>
-      </c>
-      <c r="D4" s="20">
+      <c r="C4" s="22">
+        <v>1</v>
+      </c>
+      <c r="D4" s="15">
         <v>2.048</v>
       </c>
-      <c r="E4" s="20">
-        <v>1</v>
-      </c>
-      <c r="F4" s="20">
-        <v>2</v>
-      </c>
-      <c r="G4" s="20">
+      <c r="E4" s="15">
+        <v>1</v>
+      </c>
+      <c r="F4" s="15">
+        <v>2</v>
+      </c>
+      <c r="G4" s="15">
         <f t="shared" si="1"/>
         <v>2.2321428571428571E-4</v>
       </c>
-      <c r="H4" s="20">
+      <c r="H4" s="15">
         <f t="shared" si="2"/>
         <v>4.8828125E-4</v>
       </c>
-      <c r="I4" s="20">
+      <c r="I4" s="15">
         <f t="shared" si="3"/>
         <v>2.384185791015625E-4</v>
       </c>
-      <c r="T4" s="20">
+      <c r="T4" s="15">
         <v>3.274</v>
       </c>
-      <c r="U4" s="20">
+      <c r="U4" s="15">
         <v>0.99099999999999999</v>
       </c>
-      <c r="V4" s="20">
+      <c r="V4" s="15">
         <v>3.0999999999999999E-3</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A5" s="20">
+      <c r="A5" s="15">
         <v>3.4</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="15">
         <f t="shared" si="0"/>
         <v>2.125</v>
       </c>
-      <c r="C5" s="27">
-        <v>1</v>
-      </c>
-      <c r="D5" s="20">
+      <c r="C5" s="22">
+        <v>1</v>
+      </c>
+      <c r="D5" s="15">
         <v>2.048</v>
       </c>
-      <c r="E5" s="20">
-        <v>1</v>
-      </c>
-      <c r="F5" s="20">
-        <v>2</v>
-      </c>
-      <c r="G5" s="20">
+      <c r="E5" s="15">
+        <v>1</v>
+      </c>
+      <c r="F5" s="15">
+        <v>2</v>
+      </c>
+      <c r="G5" s="15">
         <f t="shared" si="1"/>
         <v>2.2977941176470588E-4</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H5" s="15">
         <f t="shared" si="2"/>
         <v>4.8828125E-4</v>
       </c>
-      <c r="I5" s="20">
+      <c r="I5" s="15">
         <f t="shared" si="3"/>
         <v>2.384185791015625E-4</v>
       </c>
-      <c r="T5" s="20">
+      <c r="T5" s="15">
         <v>3.4</v>
       </c>
-      <c r="U5" s="20">
+      <c r="U5" s="15">
         <v>0.99099999999999999</v>
       </c>
-      <c r="V5" s="20">
+      <c r="V5" s="15">
         <v>3.2000000000000002E-3</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A6" s="20">
+      <c r="A6" s="15">
         <v>3.3</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="15">
         <f t="shared" si="0"/>
         <v>2.0624999999999996</v>
       </c>
-      <c r="C6" s="27">
-        <v>1</v>
-      </c>
-      <c r="D6" s="20">
+      <c r="C6" s="22">
+        <v>1</v>
+      </c>
+      <c r="D6" s="15">
         <v>2.048</v>
       </c>
-      <c r="E6" s="20">
-        <v>1</v>
-      </c>
-      <c r="F6" s="20">
-        <v>2</v>
-      </c>
-      <c r="G6" s="20">
+      <c r="E6" s="15">
+        <v>1</v>
+      </c>
+      <c r="F6" s="15">
+        <v>2</v>
+      </c>
+      <c r="G6" s="15">
         <f t="shared" si="1"/>
         <v>2.367424242424243E-4</v>
       </c>
-      <c r="H6" s="20">
+      <c r="H6" s="15">
         <f t="shared" si="2"/>
         <v>4.8828125E-4</v>
       </c>
-      <c r="I6" s="20">
+      <c r="I6" s="15">
         <f t="shared" si="3"/>
         <v>2.384185791015625E-4</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A7" s="20">
+      <c r="A7" s="15">
         <v>3.2</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="C7" s="27">
-        <v>1</v>
-      </c>
-      <c r="D7" s="20">
+      <c r="C7" s="22">
+        <v>1</v>
+      </c>
+      <c r="D7" s="15">
         <v>2.048</v>
       </c>
-      <c r="E7" s="20">
-        <v>1</v>
-      </c>
-      <c r="F7" s="20">
-        <v>2</v>
-      </c>
-      <c r="G7" s="20">
+      <c r="E7" s="15">
+        <v>1</v>
+      </c>
+      <c r="F7" s="15">
+        <v>2</v>
+      </c>
+      <c r="G7" s="15">
         <f t="shared" si="1"/>
         <v>2.44140625E-4</v>
       </c>
-      <c r="H7" s="20">
+      <c r="H7" s="15">
         <f t="shared" si="2"/>
         <v>4.8828125E-4</v>
       </c>
-      <c r="I7" s="20">
+      <c r="I7" s="15">
         <f t="shared" si="3"/>
         <v>2.384185791015625E-4</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A8" s="20">
+      <c r="A8" s="15">
         <v>3.1</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B8" s="22">
         <f t="shared" si="0"/>
         <v>1.9375</v>
       </c>
-      <c r="C8" s="27">
-        <v>1</v>
-      </c>
-      <c r="D8" s="20">
+      <c r="C8" s="22">
+        <v>1</v>
+      </c>
+      <c r="D8" s="15">
         <v>2.048</v>
       </c>
-      <c r="E8" s="20">
-        <v>1</v>
-      </c>
-      <c r="F8" s="20">
-        <v>2</v>
-      </c>
-      <c r="G8" s="20">
+      <c r="E8" s="15">
+        <v>1</v>
+      </c>
+      <c r="F8" s="15">
+        <v>2</v>
+      </c>
+      <c r="G8" s="15">
         <f t="shared" si="1"/>
         <v>2.5201612903225806E-4</v>
       </c>
-      <c r="H8" s="20">
+      <c r="H8" s="15">
         <f t="shared" si="2"/>
         <v>4.8828125E-4</v>
       </c>
-      <c r="I8" s="20">
+      <c r="I8" s="15">
         <f t="shared" si="3"/>
         <v>2.384185791015625E-4</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A9" s="20">
+      <c r="A9" s="15">
         <v>3</v>
       </c>
-      <c r="B9" s="27">
+      <c r="B9" s="22">
         <f t="shared" si="0"/>
         <v>1.875</v>
       </c>
-      <c r="C9" s="27">
-        <v>1</v>
-      </c>
-      <c r="D9" s="20">
+      <c r="C9" s="22">
+        <v>1</v>
+      </c>
+      <c r="D9" s="15">
         <v>2.048</v>
       </c>
-      <c r="E9" s="20">
-        <v>1</v>
-      </c>
-      <c r="F9" s="20">
-        <v>2</v>
-      </c>
-      <c r="G9" s="20">
+      <c r="E9" s="15">
+        <v>1</v>
+      </c>
+      <c r="F9" s="15">
+        <v>2</v>
+      </c>
+      <c r="G9" s="15">
         <f t="shared" si="1"/>
         <v>2.6041666666666666E-4</v>
       </c>
-      <c r="H9" s="20">
+      <c r="H9" s="15">
         <f t="shared" si="2"/>
         <v>4.8828125E-4</v>
       </c>
-      <c r="I9" s="20">
+      <c r="I9" s="15">
         <f t="shared" si="3"/>
         <v>2.384185791015625E-4</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A10" s="20">
+      <c r="A10" s="15">
         <v>2.9</v>
       </c>
-      <c r="B10" s="27">
+      <c r="B10" s="22">
         <f t="shared" si="0"/>
         <v>1.8124999999999998</v>
       </c>
-      <c r="C10" s="27">
-        <v>1</v>
-      </c>
-      <c r="D10" s="20">
+      <c r="C10" s="22">
+        <v>1</v>
+      </c>
+      <c r="D10" s="15">
         <v>2.048</v>
       </c>
-      <c r="E10" s="20">
-        <v>1</v>
-      </c>
-      <c r="F10" s="20">
-        <v>2</v>
-      </c>
-      <c r="G10" s="20">
+      <c r="E10" s="15">
+        <v>1</v>
+      </c>
+      <c r="F10" s="15">
+        <v>2</v>
+      </c>
+      <c r="G10" s="15">
         <f t="shared" si="1"/>
         <v>2.6939655172413798E-4</v>
       </c>
-      <c r="H10" s="20">
+      <c r="H10" s="15">
         <f t="shared" si="2"/>
         <v>4.8828125E-4</v>
       </c>
-      <c r="I10" s="20">
+      <c r="I10" s="15">
         <f t="shared" si="3"/>
         <v>2.384185791015625E-4</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A11" s="20">
+      <c r="A11" s="15">
         <v>2.8</v>
       </c>
-      <c r="B11" s="27">
+      <c r="B11" s="22">
         <f t="shared" si="0"/>
         <v>1.7499999999999998</v>
       </c>
-      <c r="C11" s="27">
-        <v>1</v>
-      </c>
-      <c r="D11" s="20">
+      <c r="C11" s="22">
+        <v>1</v>
+      </c>
+      <c r="D11" s="15">
         <v>2.048</v>
       </c>
-      <c r="E11" s="20">
-        <v>1</v>
-      </c>
-      <c r="F11" s="20">
-        <v>2</v>
-      </c>
-      <c r="G11" s="20">
+      <c r="E11" s="15">
+        <v>1</v>
+      </c>
+      <c r="F11" s="15">
+        <v>2</v>
+      </c>
+      <c r="G11" s="15">
         <f t="shared" si="1"/>
         <v>2.7901785714285718E-4</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="15">
         <f t="shared" si="2"/>
         <v>4.8828125E-4</v>
       </c>
-      <c r="I11" s="20">
+      <c r="I11" s="15">
         <f t="shared" si="3"/>
         <v>2.384185791015625E-4</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A12" s="20">
+      <c r="A12" s="15">
         <v>2.7</v>
       </c>
-      <c r="B12" s="27">
+      <c r="B12" s="22">
         <f t="shared" si="0"/>
         <v>1.6875</v>
       </c>
-      <c r="C12" s="27">
-        <v>1</v>
-      </c>
-      <c r="D12" s="20">
+      <c r="C12" s="22">
+        <v>1</v>
+      </c>
+      <c r="D12" s="15">
         <v>2.048</v>
       </c>
-      <c r="E12" s="20">
-        <v>1</v>
-      </c>
-      <c r="F12" s="20">
-        <v>2</v>
-      </c>
-      <c r="G12" s="20">
+      <c r="E12" s="15">
+        <v>1</v>
+      </c>
+      <c r="F12" s="15">
+        <v>2</v>
+      </c>
+      <c r="G12" s="15">
         <f t="shared" si="1"/>
         <v>2.8935185185185184E-4</v>
       </c>
-      <c r="H12" s="20">
+      <c r="H12" s="15">
         <f t="shared" si="2"/>
         <v>4.8828125E-4</v>
       </c>
-      <c r="I12" s="20">
+      <c r="I12" s="15">
         <f t="shared" si="3"/>
         <v>2.384185791015625E-4</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A13" s="20">
+      <c r="A13" s="15">
         <v>2.6</v>
       </c>
-      <c r="B13" s="27">
+      <c r="B13" s="22">
         <f t="shared" si="0"/>
         <v>1.625</v>
       </c>
-      <c r="C13" s="27">
-        <v>1</v>
-      </c>
-      <c r="D13" s="20">
+      <c r="C13" s="22">
+        <v>1</v>
+      </c>
+      <c r="D13" s="15">
         <v>2.048</v>
       </c>
-      <c r="E13" s="20">
-        <v>1</v>
-      </c>
-      <c r="F13" s="20">
-        <v>2</v>
-      </c>
-      <c r="G13" s="20">
+      <c r="E13" s="15">
+        <v>1</v>
+      </c>
+      <c r="F13" s="15">
+        <v>2</v>
+      </c>
+      <c r="G13" s="15">
         <f t="shared" si="1"/>
         <v>3.0048076923076925E-4</v>
       </c>
-      <c r="H13" s="20">
+      <c r="H13" s="15">
         <f t="shared" si="2"/>
         <v>4.8828125E-4</v>
       </c>
-      <c r="I13" s="20">
+      <c r="I13" s="15">
         <f t="shared" si="3"/>
         <v>2.384185791015625E-4</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A14" s="20">
+      <c r="A14" s="15">
         <v>2.5</v>
       </c>
-      <c r="B14" s="27">
+      <c r="B14" s="22">
         <f t="shared" si="0"/>
         <v>1.5625</v>
       </c>
-      <c r="C14" s="27">
-        <v>1</v>
-      </c>
-      <c r="D14" s="20">
+      <c r="C14" s="22">
+        <v>1</v>
+      </c>
+      <c r="D14" s="15">
         <v>2.048</v>
       </c>
-      <c r="E14" s="20">
-        <v>1</v>
-      </c>
-      <c r="F14" s="20">
-        <v>2</v>
-      </c>
-      <c r="G14" s="20">
+      <c r="E14" s="15">
+        <v>1</v>
+      </c>
+      <c r="F14" s="15">
+        <v>2</v>
+      </c>
+      <c r="G14" s="15">
         <f t="shared" si="1"/>
         <v>3.1250000000000001E-4</v>
       </c>
-      <c r="H14" s="20">
+      <c r="H14" s="15">
         <f t="shared" si="2"/>
         <v>4.8828125E-4</v>
       </c>
-      <c r="I14" s="20">
+      <c r="I14" s="15">
         <f t="shared" si="3"/>
         <v>2.384185791015625E-4</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A15" s="20">
+      <c r="A15" s="15">
         <v>2.4</v>
       </c>
-      <c r="B15" s="27">
+      <c r="B15" s="22">
         <f t="shared" si="0"/>
         <v>1.4999999999999998</v>
       </c>
-      <c r="C15" s="27">
-        <v>1</v>
-      </c>
-      <c r="D15" s="20">
+      <c r="C15" s="22">
+        <v>1</v>
+      </c>
+      <c r="D15" s="15">
         <v>2.048</v>
       </c>
-      <c r="E15" s="20">
-        <v>1</v>
-      </c>
-      <c r="F15" s="20">
-        <v>2</v>
-      </c>
-      <c r="G15" s="20">
+      <c r="E15" s="15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="15">
+        <v>2</v>
+      </c>
+      <c r="G15" s="15">
         <f t="shared" si="1"/>
         <v>3.2552083333333337E-4</v>
       </c>
-      <c r="H15" s="20">
+      <c r="H15" s="15">
         <f t="shared" si="2"/>
         <v>4.8828125E-4</v>
       </c>
-      <c r="I15" s="20">
+      <c r="I15" s="15">
         <f t="shared" si="3"/>
         <v>2.384185791015625E-4</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.45">
-      <c r="A16" s="20">
+      <c r="A16" s="15">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B16" s="27">
+      <c r="B16" s="22">
         <f t="shared" si="0"/>
         <v>1.4374999999999998</v>
       </c>
-      <c r="C16" s="27">
-        <v>1</v>
-      </c>
-      <c r="D16" s="20">
+      <c r="C16" s="22">
+        <v>1</v>
+      </c>
+      <c r="D16" s="15">
         <v>2.048</v>
       </c>
-      <c r="E16" s="20">
-        <v>1</v>
-      </c>
-      <c r="F16" s="20">
-        <v>2</v>
-      </c>
-      <c r="G16" s="20">
+      <c r="E16" s="15">
+        <v>1</v>
+      </c>
+      <c r="F16" s="15">
+        <v>2</v>
+      </c>
+      <c r="G16" s="15">
         <f t="shared" si="1"/>
         <v>3.3967391304347831E-4</v>
       </c>
-      <c r="H16" s="20">
+      <c r="H16" s="15">
         <f t="shared" si="2"/>
         <v>4.8828125E-4</v>
       </c>
-      <c r="I16" s="20">
+      <c r="I16" s="15">
         <f t="shared" si="3"/>
         <v>2.384185791015625E-4</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A17" s="20">
+      <c r="A17" s="15">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B17" s="27">
+      <c r="B17" s="22">
         <f t="shared" si="0"/>
         <v>1.375</v>
       </c>
-      <c r="C17" s="27">
-        <v>1</v>
-      </c>
-      <c r="D17" s="27">
-        <v>2</v>
-      </c>
-      <c r="E17" s="20">
-        <v>1</v>
-      </c>
-      <c r="F17" s="20">
-        <v>2</v>
-      </c>
-      <c r="G17" s="20">
+      <c r="C17" s="22">
+        <v>1</v>
+      </c>
+      <c r="D17" s="22">
+        <v>2</v>
+      </c>
+      <c r="E17" s="15">
+        <v>1</v>
+      </c>
+      <c r="F17" s="15">
+        <v>2</v>
+      </c>
+      <c r="G17" s="15">
         <f t="shared" si="1"/>
         <v>3.5511363636363637E-4</v>
       </c>
-      <c r="H17" s="20">
+      <c r="H17" s="15">
         <f t="shared" si="2"/>
         <v>4.8828125E-4</v>
       </c>
-      <c r="I17" s="20">
+      <c r="I17" s="15">
         <f t="shared" si="3"/>
         <v>2.44140625E-4</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A21" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>185</v>
+      <c r="A21" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A22" s="20" t="s">
-        <v>189</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>190</v>
+      <c r="A22" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>